<commit_message>
Adjusted some prices and added Carandash Wooden boxes
</commit_message>
<xml_diff>
--- a/Sint Promo Lijst.xlsx
+++ b/Sint Promo Lijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomvanschoor/Projects/Personal/artstory/artstory-data-sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9D47A8-4884-9140-A93C-7CE7FC7C5093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C10630-F2BF-1A46-AFE7-400B51275B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="23260" windowHeight="12460" xr2:uid="{425370B8-88E7-40A4-B4C0-702328F35FC8}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t>Brand</t>
   </si>
@@ -138,9 +138,6 @@
     <t xml:space="preserve">Multimedia Kleurboek Odelia Gardens </t>
   </si>
   <si>
-    <t>Aquaplus - Aquarelverf set rood - 12</t>
-  </si>
-  <si>
     <t>ColourPlus set an 24 Kleurpotloden</t>
   </si>
   <si>
@@ -256,6 +253,21 @@
   </si>
   <si>
     <t>Clairfontaine</t>
+  </si>
+  <si>
+    <t>Aquaplus - Aquarelverf set rood of blauw- 12</t>
+  </si>
+  <si>
+    <t>Classic Pablo Houten Kist 120 Stuks Kleurpotloden-FSC</t>
+  </si>
+  <si>
+    <t>Classic Supracolor Houten Kist - 120 Stuks Aquarel Kleurpotloden-FSC</t>
+  </si>
+  <si>
+    <t>Classic Neocolor II Houten Kist - 84 Stuks - Aquarel Pastel</t>
+  </si>
+  <si>
+    <t>Classic Supracolor Houten Kist - 80 Stuks Aquarel Kleurpotloden-FSC</t>
   </si>
 </sst>
 </file>
@@ -687,10 +699,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3FAC6E-6F54-4978-AA1E-98D2FEDD2C63}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -709,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -721,7 +733,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -741,6 +753,7 @@
         <v>5.3</v>
       </c>
       <c r="F2" s="9">
+        <f>E2/D2*100-100</f>
         <v>-18.461538461538467</v>
       </c>
     </row>
@@ -761,6 +774,7 @@
         <v>3.5</v>
       </c>
       <c r="F3" s="9">
+        <f t="shared" ref="F3:F42" si="0">E3/D3*100-100</f>
         <v>-43.089430894308947</v>
       </c>
     </row>
@@ -781,6 +795,7 @@
         <v>4.25</v>
       </c>
       <c r="F4" s="9">
+        <f t="shared" si="0"/>
         <v>-45.161290322580648</v>
       </c>
     </row>
@@ -798,10 +813,11 @@
         <v>4.95</v>
       </c>
       <c r="E5" s="8">
-        <v>2.5299999999999998</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F5" s="9">
-        <v>-48.888888888888893</v>
+        <f t="shared" si="0"/>
+        <v>-48.484848484848484</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -821,6 +837,7 @@
         <v>6.5</v>
       </c>
       <c r="F6" s="9">
+        <f t="shared" si="0"/>
         <v>-34.93493493493493</v>
       </c>
     </row>
@@ -841,6 +858,7 @@
         <v>4.25</v>
       </c>
       <c r="F7" s="9">
+        <f t="shared" si="0"/>
         <v>-34.615384615384613</v>
       </c>
     </row>
@@ -861,6 +879,7 @@
         <v>4.7</v>
       </c>
       <c r="F8" s="9">
+        <f t="shared" si="0"/>
         <v>-45.348837209302317</v>
       </c>
     </row>
@@ -881,6 +900,7 @@
         <v>5.25</v>
       </c>
       <c r="F9" s="9">
+        <f t="shared" si="0"/>
         <v>-34.292866082603254</v>
       </c>
     </row>
@@ -901,6 +921,7 @@
         <v>5.25</v>
       </c>
       <c r="F10" s="9">
+        <f t="shared" si="0"/>
         <v>-34.292866082603254</v>
       </c>
     </row>
@@ -918,10 +939,11 @@
         <v>10.25</v>
       </c>
       <c r="E11" s="8">
-        <v>5.55</v>
+        <v>5.6</v>
       </c>
       <c r="F11" s="9">
-        <v>-45.853658536585364</v>
+        <f t="shared" si="0"/>
+        <v>-45.365853658536594</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -938,10 +960,11 @@
         <v>12.05</v>
       </c>
       <c r="E12" s="8">
-        <v>6.5</v>
+        <v>6.8</v>
       </c>
       <c r="F12" s="9">
-        <v>-46.058091286307054</v>
+        <f t="shared" si="0"/>
+        <v>-43.568464730290458</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -961,12 +984,13 @@
         <v>43.5</v>
       </c>
       <c r="F13" s="9">
+        <f t="shared" si="0"/>
         <v>-20.894708128750679</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>26</v>
@@ -981,12 +1005,13 @@
         <v>7.85</v>
       </c>
       <c r="F14" s="9">
+        <f t="shared" si="0"/>
         <v>-44.718309859154928</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>28</v>
@@ -1001,12 +1026,13 @@
         <v>7.85</v>
       </c>
       <c r="F15" s="9">
+        <f t="shared" si="0"/>
         <v>-44.718309859154928</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>30</v>
@@ -1021,18 +1047,19 @@
         <v>7.85</v>
       </c>
       <c r="F16" s="9">
+        <f t="shared" si="0"/>
         <v>-44.718309859154928</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="7">
         <v>1222609</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="D17" s="8">
         <v>6.4</v>
@@ -1041,18 +1068,19 @@
         <v>4.8</v>
       </c>
       <c r="F17" s="9">
+        <f t="shared" si="0"/>
         <v>-25.000000000000014</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18" s="7">
         <v>1233469</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="8">
         <v>8.3000000000000007</v>
@@ -1061,39 +1089,41 @@
         <v>6.05</v>
       </c>
       <c r="F18" s="9">
+        <f t="shared" si="0"/>
         <v>-27.108433734939766</v>
       </c>
       <c r="N18" s="1"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>35</v>
-      </c>
       <c r="D19" s="8">
+        <v>12.9</v>
+      </c>
+      <c r="E19" s="8">
         <v>8.75</v>
       </c>
-      <c r="E19" s="8">
-        <v>12.9</v>
-      </c>
       <c r="F19" s="9">
-        <v>47.428571428571445</v>
+        <f t="shared" si="0"/>
+        <v>-32.170542635658919</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="10">
         <v>666312</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="8">
         <v>32</v>
@@ -1102,18 +1132,19 @@
         <v>20.95</v>
       </c>
       <c r="F20" s="9">
+        <f t="shared" si="0"/>
         <v>-34.53125</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="10">
         <v>186315</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="8">
         <v>37</v>
@@ -1122,18 +1153,19 @@
         <v>24</v>
       </c>
       <c r="F21" s="9">
+        <f t="shared" si="0"/>
         <v>-35.13513513513513</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="10">
         <v>1000315</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="8">
         <v>44</v>
@@ -1142,18 +1174,19 @@
         <v>28.5</v>
       </c>
       <c r="F22" s="9">
+        <f t="shared" si="0"/>
         <v>-35.227272727272734</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="7">
         <v>60325012</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="8">
         <v>10.6</v>
@@ -1162,18 +1195,19 @@
         <v>6.4</v>
       </c>
       <c r="F23" s="9">
+        <f t="shared" si="0"/>
         <v>-39.622641509433954</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="7">
         <v>60121250</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="8">
         <v>12.4</v>
@@ -1182,6 +1216,7 @@
         <v>8.1</v>
       </c>
       <c r="F24" s="9">
+        <f t="shared" si="0"/>
         <v>-34.677419354838719</v>
       </c>
     </row>
@@ -1193,7 +1228,7 @@
         <v>16550001</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="8">
         <v>29.95</v>
@@ -1202,6 +1237,7 @@
         <v>19.5</v>
       </c>
       <c r="F25" s="9">
+        <f t="shared" si="0"/>
         <v>-34.891485809682791</v>
       </c>
     </row>
@@ -1213,7 +1249,7 @@
         <v>16550002</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D26" s="8">
         <v>18.55</v>
@@ -1222,6 +1258,7 @@
         <v>12.95</v>
       </c>
       <c r="F26" s="9">
+        <f t="shared" si="0"/>
         <v>-30.188679245283026</v>
       </c>
     </row>
@@ -1230,10 +1267,10 @@
         <v>7</v>
       </c>
       <c r="B27" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="D27" s="8">
         <v>7.95</v>
@@ -1242,6 +1279,7 @@
         <v>5.15</v>
       </c>
       <c r="F27" s="9">
+        <f t="shared" si="0"/>
         <v>-35.220125786163521</v>
       </c>
     </row>
@@ -1250,10 +1288,10 @@
         <v>7</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" s="8">
         <v>7.95</v>
@@ -1262,6 +1300,7 @@
         <v>5.15</v>
       </c>
       <c r="F28" s="9">
+        <f t="shared" si="0"/>
         <v>-35.220125786163521</v>
       </c>
     </row>
@@ -1270,10 +1309,10 @@
         <v>7</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D29" s="8">
         <v>7.95</v>
@@ -1282,18 +1321,19 @@
         <v>5.15</v>
       </c>
       <c r="F29" s="9">
+        <f t="shared" si="0"/>
         <v>-35.220125786163521</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" s="11">
         <v>563830</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D30" s="8">
         <v>24.99</v>
@@ -1302,18 +1342,19 @@
         <v>22.5</v>
       </c>
       <c r="F30" s="9">
+        <f t="shared" si="0"/>
         <v>-9.963985594237684</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" s="8">
         <v>29.99</v>
@@ -1322,18 +1363,19 @@
         <v>21.95</v>
       </c>
       <c r="F31" s="9">
+        <f t="shared" si="0"/>
         <v>-26.808936312104038</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D32" s="8">
         <v>29.99</v>
@@ -1342,6 +1384,7 @@
         <v>21.95</v>
       </c>
       <c r="F32" s="9">
+        <f t="shared" si="0"/>
         <v>-26.808936312104038</v>
       </c>
     </row>
@@ -1350,10 +1393,10 @@
         <v>23</v>
       </c>
       <c r="B33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="D33" s="8">
         <v>28.99</v>
@@ -1362,6 +1405,7 @@
         <v>25.99</v>
       </c>
       <c r="F33" s="9">
+        <f t="shared" si="0"/>
         <v>-10.348395998620219</v>
       </c>
     </row>
@@ -1370,10 +1414,10 @@
         <v>23</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="D34" s="8">
         <v>28.99</v>
@@ -1382,18 +1426,19 @@
         <v>25.99</v>
       </c>
       <c r="F34" s="9">
+        <f t="shared" si="0"/>
         <v>-10.348395998620219</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="12">
         <v>2190614</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D35" s="8">
         <v>86.4</v>
@@ -1402,18 +1447,19 @@
         <v>51.85</v>
       </c>
       <c r="F35" s="9">
+        <f t="shared" si="0"/>
         <v>-39.988425925925931</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B36" s="7">
         <v>1820310</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" s="8">
         <v>74.25</v>
@@ -1422,18 +1468,19 @@
         <v>40.950000000000003</v>
       </c>
       <c r="F36" s="9">
+        <f t="shared" si="0"/>
         <v>-44.848484848484851</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B37" s="13">
         <v>31823032</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D37" s="8">
         <v>64.05</v>
@@ -1442,18 +1489,19 @@
         <v>41.5</v>
       </c>
       <c r="F37" s="9">
+        <f t="shared" si="0"/>
         <v>-35.206869633099132</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="7">
         <v>31823116</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D38" s="8">
         <v>45.2</v>
@@ -1462,7 +1510,92 @@
         <v>29.6</v>
       </c>
       <c r="F38" s="9">
+        <f t="shared" si="0"/>
         <v>-34.513274336283189</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="7">
+        <v>666920</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="8">
+        <v>459</v>
+      </c>
+      <c r="E39" s="8">
+        <v>299</v>
+      </c>
+      <c r="F39" s="9">
+        <f t="shared" si="0"/>
+        <v>-34.858387799564269</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="7">
+        <v>3888920</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" s="8">
+        <v>459</v>
+      </c>
+      <c r="E40" s="8">
+        <v>299</v>
+      </c>
+      <c r="F40" s="9">
+        <f t="shared" si="0"/>
+        <v>-34.858387799564269</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="7">
+        <v>7500484</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" s="8">
+        <v>365</v>
+      </c>
+      <c r="E41" s="8">
+        <v>250</v>
+      </c>
+      <c r="F41" s="9">
+        <f t="shared" si="0"/>
+        <v>-31.506849315068493</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" s="7">
+        <v>3888480</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D42" s="8">
+        <v>355</v>
+      </c>
+      <c r="E42" s="8">
+        <v>239</v>
+      </c>
+      <c r="F42" s="9">
+        <f t="shared" si="0"/>
+        <v>-32.676056338028175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed some products from caps to title case.
</commit_message>
<xml_diff>
--- a/Sint Promo Lijst.xlsx
+++ b/Sint Promo Lijst.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomvanschoor/Projects/Personal/artstory/artstory-data-sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C10630-F2BF-1A46-AFE7-400B51275B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5062B980-4072-4E4D-B24B-E1695184CD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="23260" windowHeight="12460" xr2:uid="{425370B8-88E7-40A4-B4C0-702328F35FC8}"/>
   </bookViews>
@@ -153,15 +153,6 @@
     <t>Caran d'Ache</t>
   </si>
   <si>
-    <t>CLASSIC PABLO PENC. ASS.12PCS-FSC</t>
-  </si>
-  <si>
-    <t>CLASSIC FIBRALO BRUSH ASSORTIMENT 15PCS</t>
-  </si>
-  <si>
-    <t>GOUACHE CAKES ASSORTED 15PCS</t>
-  </si>
-  <si>
     <t>Creatives Fineliner Brush pen set 12 kleuren</t>
   </si>
   <si>
@@ -255,9 +246,6 @@
     <t>Clairfontaine</t>
   </si>
   <si>
-    <t>Aquaplus - Aquarelverf set rood of blauw- 12</t>
-  </si>
-  <si>
     <t>Classic Pablo Houten Kist 120 Stuks Kleurpotloden-FSC</t>
   </si>
   <si>
@@ -268,6 +256,18 @@
   </si>
   <si>
     <t>Classic Supracolor Houten Kist - 80 Stuks Aquarel Kleurpotloden-FSC</t>
+  </si>
+  <si>
+    <t>Aquaplus - Aquarelverf set rood of blauw - 12</t>
+  </si>
+  <si>
+    <t>Classic Pablo Kleurpotloden - 12 Stuks - FSC</t>
+  </si>
+  <si>
+    <t>Classic Fibralo Brushstiften Assortiment - 15 Stuks</t>
+  </si>
+  <si>
+    <t>Gouache Cakes Assortiment - 15 Stuks</t>
   </si>
 </sst>
 </file>
@@ -701,8 +701,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -721,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -733,7 +733,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -990,7 +990,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>26</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>28</v>
@@ -1032,7 +1032,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>30</v>
@@ -1059,7 +1059,7 @@
         <v>1222609</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D17" s="8">
         <v>6.4</v>
@@ -1123,7 +1123,7 @@
         <v>666312</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="D20" s="8">
         <v>32</v>
@@ -1144,7 +1144,7 @@
         <v>186315</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="D21" s="8">
         <v>37</v>
@@ -1165,7 +1165,7 @@
         <v>1000315</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="D22" s="8">
         <v>44</v>
@@ -1180,13 +1180,13 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B23" s="7">
         <v>60325012</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D23" s="8">
         <v>10.6</v>
@@ -1201,13 +1201,13 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24" s="7">
         <v>60121250</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D24" s="8">
         <v>12.4</v>
@@ -1228,7 +1228,7 @@
         <v>16550001</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D25" s="8">
         <v>29.95</v>
@@ -1249,7 +1249,7 @@
         <v>16550002</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D26" s="8">
         <v>18.55</v>
@@ -1267,10 +1267,10 @@
         <v>7</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D27" s="8">
         <v>7.95</v>
@@ -1288,10 +1288,10 @@
         <v>7</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D28" s="8">
         <v>7.95</v>
@@ -1309,10 +1309,10 @@
         <v>7</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D29" s="8">
         <v>7.95</v>
@@ -1327,13 +1327,13 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B30" s="11">
         <v>563830</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D30" s="8">
         <v>24.99</v>
@@ -1348,13 +1348,13 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D31" s="8">
         <v>29.99</v>
@@ -1369,13 +1369,13 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D32" s="8">
         <v>29.99</v>
@@ -1393,10 +1393,10 @@
         <v>23</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D33" s="8">
         <v>28.99</v>
@@ -1414,10 +1414,10 @@
         <v>23</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D34" s="8">
         <v>28.99</v>
@@ -1432,13 +1432,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B35" s="12">
         <v>2190614</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D35" s="8">
         <v>86.4</v>
@@ -1453,13 +1453,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B36" s="7">
         <v>1820310</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D36" s="8">
         <v>74.25</v>
@@ -1474,13 +1474,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B37" s="13">
         <v>31823032</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D37" s="8">
         <v>64.05</v>
@@ -1495,13 +1495,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B38" s="7">
         <v>31823116</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D38" s="8">
         <v>45.2</v>
@@ -1522,7 +1522,7 @@
         <v>666920</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D39" s="8">
         <v>459</v>
@@ -1543,7 +1543,7 @@
         <v>3888920</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D40" s="8">
         <v>459</v>
@@ -1564,7 +1564,7 @@
         <v>7500484</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D41" s="8">
         <v>365</v>
@@ -1585,7 +1585,7 @@
         <v>3888480</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D42" s="8">
         <v>355</v>

</xml_diff>